<commit_message>
Finalised and generated Gerbers.
</commit_message>
<xml_diff>
--- a/Other/Sensor BOM.xlsx
+++ b/Other/Sensor BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/University Shit/3rd Year/1st Sem/EEE3088F/EEE3088F-Team-9/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7327BE80-FD7B-9B4A-A0F7-677CA3FDF1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D849977-A719-8F47-8AE3-435981D1DE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{04BB928B-835B-6640-9E3B-3EA0554ADE48}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>$0.04215</t>
   </si>
   <si>
-    <t>$0.033</t>
-  </si>
-  <si>
     <t>$13.443</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Grand Total:</t>
   </si>
   <si>
-    <t>$18.61115</t>
-  </si>
-  <si>
     <t>$0.00843</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>$1.0186</t>
+  </si>
+  <si>
+    <t>$0.0055</t>
+  </si>
+  <si>
+    <t>$18.58365</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5623EA9-6C5E-EF49-9A12-EB7F35D5F042}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +560,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
@@ -571,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -586,10 +586,10 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -609,10 +609,10 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -632,18 +632,18 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>